<commit_message>
bento scripts for select by cases facet over
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_TumorGrade-HighGrade.xlsx
+++ b/InputFiles/TC01_Bento_Filter_TumorGrade-HighGrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA39C612-A757-4076-9A53-4A56BEDBFB63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC64187-56C5-44E7-9926-36E3FA9D7570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+          WHERE   d.tumor_grade IN ["High Grade"] 
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
+MATCH (samp)&lt;-[:file_of_sample]-(f)
+MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
+RETURN COUNT(DISTINCT p) AS Programs,
+COUNT(DISTINCT s) AS Arms,
+COUNT(DISTINCT ss) AS Cases,
+COUNT(DISTINCT samp) AS Samples,
+COUNT(DISTINCT lp) AS Assays,
+COUNT(DISTINCT f) AS Files</t>
+  </si>
+  <si>
+    <t>MATCH (ss:study_subject)
 MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
 WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
@@ -65,7 +83,7 @@
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
 MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
- WHERE   d.tumor_grade IN ["High Grade"] 
+        WHERE   d.tumor_grade IN ["High Grade"] 
 return ss.study_subject_id as `Case ID`,
        p.program_acronym as `Program Code`,
         p.program_id as Program_ID,
@@ -77,24 +95,6 @@
        d.pr_status AS `PR Status`,
        demo.age_at_index AS `Age (years)`,
 demo.survival_time AS `Survival (days)`</t>
-  </si>
-  <si>
-    <t>MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE   d.tumor_grade IN ["High Grade"] 
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
-MATCH (samp)&lt;-[:file_of_sample]-(f)
-MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
-RETURN COUNT(DISTINCT p) AS Programs,
-COUNT(DISTINCT s) AS Arms,
-COUNT(DISTINCT ss) AS Cases,
-COUNT(DISTINCT samp) AS Samples,
-COUNT(DISTINCT lp) AS Assays,
-COUNT(DISTINCT f) AS Files</t>
   </si>
 </sst>
 </file>
@@ -466,20 +466,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.81640625" customWidth="1"/>
-    <col min="3" max="3" width="60.453125" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
     <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -496,15 +496,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>

</xml_diff>